<commit_message>
Excel Feature: partly bug fix
</commit_message>
<xml_diff>
--- a/src/test/resources/visitLinkTest.xlsx
+++ b/src/test/resources/visitLinkTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\test_version\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D887085D-83C6-4F8B-9ACC-7EB64F5B19DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44ACB72-BEFD-4FD5-BAF9-A57C9F5C3CA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="211">
   <si>
     <t>ID</t>
   </si>
@@ -657,6 +657,9 @@
   </si>
   <si>
     <t>architecturename</t>
+  </si>
+  <si>
+    <t>Ende</t>
   </si>
 </sst>
 </file>
@@ -2265,7 +2268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -2726,11 +2729,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2963,10 +2966,16 @@
       <c r="A33" s="128" t="s">
         <v>186</v>
       </c>
+      <c r="C33" s="141">
+        <v>43359</v>
+      </c>
     </row>
     <row r="34" spans="1:3" s="129" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="129" t="s">
         <v>187</v>
+      </c>
+      <c r="C34" s="129" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="130" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>